<commit_message>
Add support to handle with missing data in profile formatters. Perform the validation of entities in service instead of batch repository. Change the batch repositories and respective service tests. Change the validation of profiles when storing, to verify if the referenced alleles exists instead of creating if not existent. Add the specification and implementation of profile tests. Change mediatype of file responses to text/plain. Add more controller tests. Perform adjusments and bug fixes
</commit_message>
<xml_diff>
--- a/docs/test cases/allele/AlleleRepositoryTests.xlsx
+++ b/docs/test cases/allele/AlleleRepositoryTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Projeto\PhyloDB\docs\test cases\allele\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E9DA11-61C0-451A-B36F-B518EF361661}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01D9FCB-21A1-4F38-8D16-F1B1E7698A6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="74">
   <si>
     <t>Parameter</t>
   </si>
@@ -213,18 +213,12 @@
     <t>alleles</t>
   </si>
   <si>
-    <t>flag</t>
-  </si>
-  <si>
     <t>project</t>
   </si>
   <si>
     <t>saved</t>
   </si>
   <si>
-    <t>skip, update</t>
-  </si>
-  <si>
     <t>p, null</t>
   </si>
   <si>
@@ -237,22 +231,28 @@
     <t xml:space="preserve"> - </t>
   </si>
   <si>
-    <t>skip</t>
-  </si>
-  <si>
     <t>nonconflict</t>
   </si>
   <si>
     <t>conflict</t>
   </si>
   <si>
-    <t>update</t>
-  </si>
-  <si>
-    <t>n-c</t>
-  </si>
-  <si>
     <t>entities</t>
+  </si>
+  <si>
+    <t>anyMissing</t>
+  </si>
+  <si>
+    <t>keys</t>
+  </si>
+  <si>
+    <t>allele</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p </t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -433,6 +433,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -445,6 +454,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -456,9 +468,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -743,20 +752,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="I127" sqref="I127"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113:XFD113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
@@ -777,7 +786,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -788,7 +797,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -797,7 +806,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -808,7 +817,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -817,7 +826,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -828,7 +837,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
@@ -837,7 +846,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -848,7 +857,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
@@ -860,11 +869,11 @@
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="7" t="s">
         <v>11</v>
       </c>
@@ -1343,7 +1352,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -1354,7 +1363,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="17"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="6" t="s">
         <v>5</v>
       </c>
@@ -1363,7 +1372,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="19" t="s">
         <v>34</v>
       </c>
       <c r="B45" s="6" t="s">
@@ -1374,7 +1383,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="17"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="6" t="s">
         <v>5</v>
       </c>
@@ -1383,7 +1392,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -1394,7 +1403,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="6" t="s">
         <v>5</v>
       </c>
@@ -1403,7 +1412,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B49" s="6" t="s">
@@ -1414,7 +1423,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="17"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="6" t="s">
         <v>5</v>
       </c>
@@ -1423,7 +1432,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="19" t="s">
         <v>57</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -1434,7 +1443,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="17"/>
+      <c r="A52" s="20"/>
       <c r="B52" s="6" t="s">
         <v>5</v>
       </c>
@@ -1443,21 +1452,21 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="21"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="25"/>
       <c r="F54" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="19"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="8" t="s">
         <v>20</v>
       </c>
@@ -1631,7 +1640,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="26" t="s">
+      <c r="A66" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B66" s="6" t="s">
@@ -1642,7 +1651,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="26"/>
+      <c r="A67" s="29"/>
       <c r="B67" s="6" t="s">
         <v>5</v>
       </c>
@@ -1651,7 +1660,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="16" t="s">
+      <c r="A68" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B68" s="6" t="s">
@@ -1662,7 +1671,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="17"/>
+      <c r="A69" s="20"/>
       <c r="B69" s="6" t="s">
         <v>5</v>
       </c>
@@ -1671,20 +1680,20 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C71" s="21"/>
+      <c r="C71" s="25"/>
       <c r="D71" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E71"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="19"/>
+      <c r="A72" s="22"/>
       <c r="B72" s="8" t="s">
         <v>20</v>
       </c>
@@ -1780,8 +1789,8 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="26" t="s">
-        <v>57</v>
+      <c r="A80" s="29" t="s">
+        <v>71</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>4</v>
@@ -1791,7 +1800,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="26"/>
+      <c r="A81" s="29"/>
       <c r="B81" s="2" t="s">
         <v>5</v>
       </c>
@@ -1800,7 +1809,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="16" t="s">
+      <c r="A82" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B82" s="6" t="s">
@@ -1811,7 +1820,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="17"/>
+      <c r="A83" s="20"/>
       <c r="B83" s="6" t="s">
         <v>5</v>
       </c>
@@ -1820,7 +1829,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="16" t="s">
+      <c r="A84" s="19" t="s">
         <v>45</v>
       </c>
       <c r="B84" s="6" t="s">
@@ -1831,7 +1840,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="17"/>
+      <c r="A85" s="20"/>
       <c r="B85" s="6" t="s">
         <v>5</v>
       </c>
@@ -1851,22 +1860,22 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="18" t="s">
+      <c r="A88" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B88" s="20" t="s">
+      <c r="B88" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C88" s="25"/>
-      <c r="D88" s="20" t="s">
+      <c r="C88" s="24"/>
+      <c r="D88" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E88" s="21"/>
+      <c r="E88" s="25"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="19"/>
+      <c r="A89" s="22"/>
       <c r="B89" s="9" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>24</v>
@@ -1884,7 +1893,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>41</v>
@@ -1902,7 +1911,7 @@
         <v>2</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>42</v>
@@ -1958,7 +1967,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="16" t="s">
+      <c r="A96" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B96" s="2" t="s">
@@ -1969,7 +1978,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="17"/>
+      <c r="A97" s="20"/>
       <c r="B97" s="2" t="s">
         <v>5</v>
       </c>
@@ -1978,7 +1987,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="16" t="s">
+      <c r="A98" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B98" s="6" t="s">
@@ -1989,7 +1998,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" s="17"/>
+      <c r="A99" s="20"/>
       <c r="B99" s="6" t="s">
         <v>5</v>
       </c>
@@ -1998,7 +2007,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="16" t="s">
+      <c r="A100" s="19" t="s">
         <v>45</v>
       </c>
       <c r="B100" s="6" t="s">
@@ -2009,7 +2018,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="17"/>
+      <c r="A101" s="20"/>
       <c r="B101" s="6" t="s">
         <v>5</v>
       </c>
@@ -2018,19 +2027,19 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="18" t="s">
+      <c r="A103" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B103" s="20" t="s">
+      <c r="B103" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C103" s="21"/>
+      <c r="C103" s="25"/>
       <c r="D103" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="19"/>
+      <c r="A104" s="22"/>
       <c r="B104" s="5" t="s">
         <v>20</v>
       </c>
@@ -2100,8 +2109,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="16" t="s">
-        <v>73</v>
+      <c r="A111" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="B111" s="12" t="s">
         <v>54</v>
@@ -2111,7 +2120,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="17"/>
+      <c r="A112" s="20"/>
       <c r="B112" s="12" t="s">
         <v>5</v>
       </c>
@@ -2119,437 +2128,466 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B113" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B117" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C117" s="24"/>
+      <c r="D117" s="25"/>
+      <c r="E117" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118" s="22"/>
+      <c r="B118" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D118" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119" s="12">
+        <v>1</v>
+      </c>
+      <c r="B119" s="12">
+        <v>0</v>
+      </c>
+      <c r="C119" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D119" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E119" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120" s="12">
+        <v>2</v>
+      </c>
+      <c r="B120" s="12">
+        <v>1</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D120" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E120" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121" s="12">
+        <v>3</v>
+      </c>
+      <c r="B121" s="12">
+        <v>1</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D121" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E121" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122" s="12">
+        <v>4</v>
+      </c>
+      <c r="B122" s="12">
+        <v>1</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D122" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E122" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123" s="14">
+        <v>5</v>
+      </c>
+      <c r="B123" s="14">
+        <v>1</v>
+      </c>
+      <c r="C123" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D123" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E123" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A124" s="14">
+        <v>6</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C124" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D124" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E124" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A125" s="14">
+        <v>7</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D125" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E125" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A126" s="14">
+        <v>8</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D126" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E126" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A127" s="14">
+        <v>9</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C127" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D127" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E127" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A129" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A130" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A131" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B131" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C131" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A132" s="20"/>
+      <c r="B132" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A133" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B133" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C133" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A134" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B134" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C113" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B114" s="12" t="s">
+      <c r="C134" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A135" s="20"/>
+      <c r="B135" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A136" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B136" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C114" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="14" t="s">
+      <c r="C136" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A137" s="20"/>
+      <c r="B137" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A139" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B139" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C139" s="24"/>
+      <c r="D139" s="25"/>
+      <c r="E139" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A140" s="22"/>
+      <c r="B140" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C140" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B115" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C115" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="14" t="s">
+      <c r="D140" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E140" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B116" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C116" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B118" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C118" s="25"/>
-      <c r="D118" s="25"/>
-      <c r="E118" s="21"/>
-      <c r="F118" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="19"/>
-      <c r="B119" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C119" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D119" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E119" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F119" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="12">
-        <v>1</v>
-      </c>
-      <c r="B120" s="12">
-        <v>0</v>
-      </c>
-      <c r="C120" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D120" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E120" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F120" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="12">
-        <v>2</v>
-      </c>
-      <c r="B121" s="12">
-        <v>1</v>
-      </c>
-      <c r="C121" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D121" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E121" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F121" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="12">
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A141" s="18">
+        <v>1</v>
+      </c>
+      <c r="B141" s="18">
+        <v>1</v>
+      </c>
+      <c r="C141" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D141" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E141" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A142" s="18">
+        <v>2</v>
+      </c>
+      <c r="B142" s="18">
+        <v>1</v>
+      </c>
+      <c r="C142" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D142" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E142" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A143" s="18">
         <v>3</v>
       </c>
-      <c r="B122" s="12">
-        <v>1</v>
-      </c>
-      <c r="C122" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D122" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E122" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F122" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" s="12">
+      <c r="B143" s="18">
+        <v>1</v>
+      </c>
+      <c r="C143" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D143" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E143" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A144" s="18">
         <v>4</v>
       </c>
-      <c r="B123" s="12">
-        <v>1</v>
-      </c>
-      <c r="C123" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D123" s="14" t="s">
+      <c r="B144" s="18">
+        <v>1</v>
+      </c>
+      <c r="C144" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D144" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E123" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F123" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="14">
+      <c r="E144" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A145" s="18">
         <v>5</v>
       </c>
-      <c r="B124" s="14">
-        <v>1</v>
-      </c>
-      <c r="C124" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D124" s="14" t="s">
+      <c r="B145" s="18">
+        <v>2</v>
+      </c>
+      <c r="C145" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D145" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E145" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A146" s="18">
+        <v>6</v>
+      </c>
+      <c r="B146" s="18">
+        <v>2</v>
+      </c>
+      <c r="C146" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D146" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E124" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F124" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A125" s="14">
-        <v>6</v>
-      </c>
-      <c r="B125" s="14">
-        <v>1</v>
-      </c>
-      <c r="C125" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D125" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E125" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F125" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" s="14">
+      <c r="E146" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A147" s="18">
         <v>7</v>
       </c>
-      <c r="B126" s="14">
-        <v>1</v>
-      </c>
-      <c r="C126" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D126" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E126" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F126" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" s="14">
-        <v>8</v>
-      </c>
-      <c r="B127" s="14">
-        <v>1</v>
-      </c>
-      <c r="C127" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D127" s="14" t="s">
+      <c r="B147" s="18">
+        <v>2</v>
+      </c>
+      <c r="C147" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D147" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E127" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F127" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="14">
-        <v>9</v>
-      </c>
-      <c r="B128" s="14">
-        <v>1</v>
-      </c>
-      <c r="C128" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D128" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E128" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F128" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129" s="14">
-        <v>10</v>
-      </c>
-      <c r="B129" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C129" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D129" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E129" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F129" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" s="14">
-        <v>11</v>
-      </c>
-      <c r="B130" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C130" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D130" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E130" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F130" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A131" s="14">
-        <v>12</v>
-      </c>
-      <c r="B131" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C131" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D131" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E131" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F131" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" s="14">
-        <v>13</v>
-      </c>
-      <c r="B132" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C132" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D132" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E132" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F132" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A133" s="14">
-        <v>14</v>
-      </c>
-      <c r="B133" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C133" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D133" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E133" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F133" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134" s="14">
-        <v>15</v>
-      </c>
-      <c r="B134" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C134" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D134" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E134" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F134" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A135" s="14">
-        <v>16</v>
-      </c>
-      <c r="B135" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C135" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D135" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E135" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F135" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A136" s="14">
-        <v>17</v>
-      </c>
-      <c r="B136" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C136" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D136" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E136" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F136" s="14" t="s">
-        <v>17</v>
+      <c r="E147" s="18" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="B118:E118"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:C88"/>
+  <mergeCells count="35">
+    <mergeCell ref="B117:D117"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A88:A89"/>
     <mergeCell ref="B54:E54"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A68:A69"/>
@@ -2560,13 +2598,21 @@
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="A47:A48"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="B139:D139"/>
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="A82:A83"/>
     <mergeCell ref="A98:A99"/>
     <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="A100:A101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>